<commit_message>
FO en User Stories aangepast
</commit_message>
<xml_diff>
--- a/documentatie/userstories.xlsx
+++ b/documentatie/userstories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA717EA-43C0-45B8-9BD4-A3BDAA7EA9E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139EBEAE-E1ED-4A9E-9D91-F34296A6935D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
   <si>
     <t>Done</t>
   </si>
@@ -118,9 +118,6 @@
     <t>In kunnen loggen</t>
   </si>
   <si>
-    <t>De site kan updaten</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
@@ -128,6 +125,18 @@
   </si>
   <si>
     <t>Medium/Large</t>
+  </si>
+  <si>
+    <t>Bij de CMS kan komen</t>
+  </si>
+  <si>
+    <t>Content kunnen toevoegen</t>
+  </si>
+  <si>
+    <t>Content kunnen aanpassen</t>
+  </si>
+  <si>
+    <t>Content kunnen verwijderen</t>
   </si>
 </sst>
 </file>
@@ -192,161 +201,7 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="75">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF1919"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0505"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB03B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9FF37"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0101"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB03B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9FF37"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0101"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB03B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9FF37"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0101"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB03B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9FF37"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0101"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB03B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9FF37"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0101"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <font>
         <color theme="0"/>
@@ -503,240 +358,6 @@
           <bgColor rgb="FFFF0101"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF1919"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0505"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB03B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9FF37"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0101"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB03B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9FF37"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0101"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB03B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9FF37"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0101"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB03B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9FF37"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0101"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB03B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9FF37"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0101"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9FF37"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB03B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB03B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00DA43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00C81D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF2ACC04"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1027,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1086,7 +707,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -1109,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -1132,7 +753,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -1155,7 +776,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -1175,7 +796,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -1195,7 +816,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -1215,7 +836,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
@@ -1235,7 +856,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>11</v>
@@ -1255,7 +876,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>11</v>
@@ -1269,96 +890,147 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
         <v>32</v>
       </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
         <v>33</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F16" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1 A3:E6 G6:XFD6 G3:G5 H2:XFD5 A2:G2 A7:XFD1048576">
-    <cfRule type="containsText" dxfId="43" priority="19" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="20" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="21" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="22" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="containsText" dxfId="39" priority="15" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="16" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="18" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="containsText" dxfId="35" priority="11" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="12" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="13" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="14" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="31" priority="7" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="8" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",F6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="6" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="containsText" dxfId="23" priority="2" operator="containsText" text="M">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="M">
       <formula>NOT(ISERROR(SEARCH("M",C15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Templates, Database, Logboek, Sprint, Userstories
Added template engine
Created CMS
Updated Logboek and user stories.
Sprint 3
Now using DB for content
</commit_message>
<xml_diff>
--- a/documentatie/userstories.xlsx
+++ b/documentatie/userstories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED60437E-87C3-46FF-8C72-870A6040BB13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA72A9C-F4B2-44EA-A1D6-1EABC95FFD33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="38">
   <si>
     <t>Done</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Content kunnen verwijderen</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -187,10 +190,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -644,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,9 +684,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
+      <c r="F2" s="3"/>
       <c r="H2" t="s">
         <v>11</v>
       </c>
@@ -727,7 +729,7 @@
         <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
@@ -773,7 +775,7 @@
         <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -793,7 +795,7 @@
         <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -847,7 +849,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>31</v>
@@ -873,7 +875,7 @@
         <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -890,7 +892,7 @@
         <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -907,7 +909,7 @@
         <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -924,7 +926,7 @@
         <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>